<commit_message>
upper and lower bounds, verplichte vrije meters goed meegenomen
</commit_message>
<xml_diff>
--- a/others/Upper and lower bound.xlsx
+++ b/others/Upper and lower bound.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vaste verhouding" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Beslissingsvariavelen</t>
   </si>
   <si>
-    <t>m vrijstand</t>
-  </si>
-  <si>
     <t>Voorwaarden</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>maisons</t>
+  </si>
+  <si>
+    <t>m EXTRA vrijstand</t>
   </si>
 </sst>
 </file>
@@ -312,15 +312,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,16 +655,16 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -689,7 +689,7 @@
         <v>8550</v>
       </c>
       <c r="G3" s="2">
-        <v>1.8232509837194708</v>
+        <v>0.5139537112127337</v>
       </c>
       <c r="H3">
         <v>285000</v>
@@ -717,7 +717,7 @@
         <v>15960</v>
       </c>
       <c r="G4" s="2">
-        <v>9.882078426251935</v>
+        <v>8.2124112433150973</v>
       </c>
       <c r="H4">
         <v>399000</v>
@@ -745,7 +745,7 @@
         <v>36600</v>
       </c>
       <c r="G5" s="2">
-        <v>31.965394035507828</v>
+        <v>29.027939463382406</v>
       </c>
       <c r="H5">
         <v>610000</v>
@@ -770,14 +770,14 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <f>SUMPRODUCT(B3:B5,C3:C5+E3:E5,D3:D5+E3:E5)</f>
         <v>8172</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
@@ -795,15 +795,15 @@
         <v>5760</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="9"/>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -817,111 +817,111 @@
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="13">
-        <v>10303757.429442272</v>
-      </c>
-      <c r="L13" s="13">
-        <v>17548757.429442272</v>
-      </c>
-      <c r="M13" s="14">
+        <v>30</v>
+      </c>
+      <c r="K13" s="11">
+        <v>9492145.1789900512</v>
+      </c>
+      <c r="L13" s="11">
+        <v>16737145.178990051</v>
+      </c>
+      <c r="M13" s="12">
         <f>L13-K13</f>
         <v>7245000</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="J14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="13">
-        <v>12613340.440967087</v>
-      </c>
-      <c r="L14" s="13">
-        <v>27103340.440967087</v>
-      </c>
-      <c r="M14" s="14">
+        <v>32</v>
+      </c>
+      <c r="K14" s="11">
+        <v>11236621.108188428</v>
+      </c>
+      <c r="L14" s="11">
+        <v>25726621.108188428</v>
+      </c>
+      <c r="M14" s="12">
         <f t="shared" ref="M14:M15" si="0">L14-K14</f>
         <v>14490000</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
         <f>SUMPRODUCT(B3:B5,F3:F5,G3:G5)</f>
-        <v>13456367.023329845</v>
+        <v>11686049.463199079</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="13">
-        <v>13456367.023329845</v>
-      </c>
-      <c r="L15" s="13">
-        <v>35191367.023329847</v>
-      </c>
-      <c r="M15" s="14">
+        <v>31</v>
+      </c>
+      <c r="K15" s="11">
+        <v>11686049.463199079</v>
+      </c>
+      <c r="L15" s="11">
+        <v>33421049.463199079</v>
+      </c>
+      <c r="M15" s="12">
         <f t="shared" si="0"/>
         <v>21735000</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7">
         <f>SUMPRODUCT(B3:B5,H3:H5)+C15</f>
-        <v>35191367.023329847</v>
+        <v>33421049.463199079</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <f>(C3+G3)*(D3+G3)-C3*D3</f>
-        <v>32.496259889145534</v>
+        <f>(C3+E3+G3)*(D3+E3+G3)-(C3+E3)*(D3+E3)</f>
+        <v>10.543222641524025</v>
       </c>
       <c r="D20">
-        <f>(C3+G3)*(D3+2*G3)-C3*D3</f>
-        <v>50.406511908535336</v>
+        <f>(C3+E3+G3)*(D3+2*E3+2*G3)-(C3+E3)*(D3+2*E3)</f>
+        <v>16.974815593346165</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
@@ -930,15 +930,15 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <f>(C4+G4)*(D4+G4)-C4*D4</f>
-        <v>270.59184648200284</v>
+        <f t="shared" ref="C21:C22" si="1">(C4+E4+G4)*(D4+E4+G4)-(C4+E4)*(D4+E4)</f>
+        <v>260.43536264723292</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D22" si="1">(C4+G4)*(D4+2*G4)-C4*D4</f>
-        <v>467.0681047671161</v>
+        <f t="shared" ref="D21:D22" si="2">(C4+E4+G4)*(D4+2*E4+2*G4)-(C4+E4)*(D4+2*E4)</f>
+        <v>459.27764096960277</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
@@ -947,15 +947,15 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <f>(C5+G5)*(D5+G5)-C5*D5</f>
-        <v>1709.0423876086977</v>
+        <f t="shared" si="1"/>
+        <v>1815.0572415131046</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>3082.448137844563</v>
+        <f t="shared" si="2"/>
+        <v>3325.3211186606941</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -970,10 +970,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -982,10 +982,10 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>(B3-E20)*C20+(B4-E21)*C21+(B5-E22)*C22+E20*D20+E21*D21+E22*D22</f>
-        <v>20628.034793736952</v>
+        <v>20628.03322137312</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26">
         <f>C12</f>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1038,16 +1038,16 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -1056,10 +1056,10 @@
       </c>
       <c r="B3">
         <f>C3*B6</f>
-        <v>0</v>
+        <v>31.864304460589029</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>0.53107174100981713</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -1106,7 +1106,7 @@
         <v>15960</v>
       </c>
       <c r="H4" s="2">
-        <v>0.34253666957885565</v>
+        <v>0.34495644935737435</v>
       </c>
       <c r="I4">
         <v>399000</v>
@@ -1118,10 +1118,10 @@
       </c>
       <c r="B5">
         <f>C5*B6</f>
-        <v>20</v>
+        <v>28.135695539410971</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>0.46892825899018287</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -1137,7 +1137,7 @@
         <v>36600</v>
       </c>
       <c r="H5" s="2">
-        <v>24.958009542704342</v>
+        <v>13.423180795805798</v>
       </c>
       <c r="I5">
         <v>610000</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="6">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <f>SUM(C3:C5)</f>
@@ -1164,7 +1164,7 @@
         <v>28800</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -1175,22 +1175,22 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <f>SUMPRODUCT(B3:B5,D3:D5+F3:F5,E3:E5+F3:F5)</f>
-        <v>5610</v>
+        <v>11078.493044863681</v>
       </c>
       <c r="J10" s="9"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1205,16 +1205,16 @@
         <v>5760</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="M11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1224,35 +1224,35 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <f>C9-C10-C11</f>
-        <v>23190</v>
+        <v>17721.506955136319</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N12" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="O12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="13">
-        <v>18269262.985259578</v>
-      </c>
-      <c r="L13" s="13">
-        <v>30469262.985259578</v>
+        <v>30</v>
+      </c>
+      <c r="K13" s="11">
+        <v>15517048.775082435</v>
+      </c>
+      <c r="L13" s="11">
+        <v>27717048.775082435</v>
       </c>
       <c r="M13" s="9">
         <v>0</v>
@@ -1263,111 +1263,111 @@
       <c r="O13" s="9">
         <v>1</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="12">
         <f>L13-K13</f>
         <v>12200000</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="J14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" s="13">
-        <v>18765324.444047619</v>
-      </c>
-      <c r="L14" s="13">
-        <v>42573748.007206976</v>
+        <v>32</v>
+      </c>
+      <c r="K14" s="11">
+        <v>15035261.688628538</v>
+      </c>
+      <c r="L14" s="11">
+        <v>36377635.198073901</v>
       </c>
       <c r="M14" s="9">
-        <v>4.550587975697247E-2</v>
+        <v>0.23520203773497222</v>
       </c>
       <c r="N14" s="9">
         <v>0</v>
       </c>
       <c r="O14" s="9">
-        <v>0.95449412024302749</v>
-      </c>
-      <c r="P14" s="14">
+        <v>0.76479796226502783</v>
+      </c>
+      <c r="P14" s="12">
         <f>L14-K14</f>
-        <v>23808423.563159358</v>
+        <v>21342373.509445362</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="5">
         <f>SUMPRODUCT(B3:B5,G3:G5,H3:H5)</f>
-        <v>18269262.985259578</v>
+        <v>13822741.326310124</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="13">
-        <v>17251995.137835562</v>
-      </c>
-      <c r="L15" s="13">
-        <v>45754572.01517725</v>
+        <v>31</v>
+      </c>
+      <c r="K15" s="11">
+        <v>13822741.326310124</v>
+      </c>
+      <c r="L15" s="11">
+        <v>40066842.376618691</v>
       </c>
       <c r="M15" s="9">
-        <v>0.41525246782863134</v>
+        <v>0.53107174100981713</v>
       </c>
       <c r="N15" s="9">
         <v>0</v>
       </c>
       <c r="O15" s="9">
-        <v>0.58474753217136866</v>
-      </c>
-      <c r="P15" s="14">
+        <v>0.46892825899018287</v>
+      </c>
+      <c r="P15" s="12">
         <f>L15-K15</f>
-        <v>28502576.877341688</v>
+        <v>26244101.050308567</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7">
         <f>SUMPRODUCT(B3:B5,I3:I5)+C15</f>
-        <v>30469262.985259578</v>
+        <v>40066842.376618691</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <f>(D3+H3)*(E3+H3)-D3*E3</f>
+        <f>(D3+F3+H3)*(E3+F3+H3)-(D3+F3)*(E3+F3)</f>
         <v>0</v>
       </c>
       <c r="D20">
-        <f>(D3+H3)*(E3+2*H3)-D3*E3</f>
+        <f>(D3+F3+H3)*(E3+2*F3+2*H3)-(D3+F3)*(E3+2*F3)</f>
         <v>0</v>
       </c>
       <c r="E20" s="2">
@@ -1377,15 +1377,15 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <f>(D4+H4)*(E4+H4)-D4*E4</f>
-        <v>6.1117230876361504</v>
+        <f t="shared" ref="C21:C22" si="0">(D4+F4+H4)*(E4+F4+H4)-(D4+F4)*(E4+F4)</f>
+        <v>8.2254715118515378</v>
       </c>
       <c r="D21">
-        <f>(D4+H4)*(E4+2*H4)-D4*E4</f>
-        <v>9.6544211534308744</v>
+        <f t="shared" ref="D21:D22" si="1">(D4+F4+H4)*(E4+2*F4+2*H4)-(D4+F4)*(E4+2*F4)</f>
+        <v>13.86376965352278</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
@@ -1394,15 +1394,15 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <f>(D5+H5)*(E5+H5)-D5*E5</f>
-        <v>1159.4994455018646</v>
+        <f t="shared" si="0"/>
+        <v>629.85833933638389</v>
       </c>
       <c r="D22">
-        <f>(D5+H5)*(E5+2*H5)-D5*E5</f>
-        <v>2056.9397908053334</v>
+        <f t="shared" si="1"/>
+        <v>1118.7732803168069</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1429,14 +1429,14 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>(B3-E20)*C20+(B4-E21)*C21+(B5-E22)*C22+E20*D20+E21*D21+E22*D22</f>
-        <v>23189.988910037289</v>
+        <v>17721.502468527498</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26">
         <f>C12</f>
-        <v>23190</v>
+        <v>17721.506955136319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>